<commit_message>
updating files to standard
</commit_message>
<xml_diff>
--- a/rnaSample/rnaSample_Brown_11.25.19.xlsx
+++ b/rnaSample/rnaSample_Brown_11.25.19.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/rnaSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FE3F8C-CA47-1143-84E1-ED4DD2E46A3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3814ADF-82A4-1148-AA5C-9D9FEC2815A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19700" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>

</xml_diff>

<commit_message>
changing FALSE to False
</commit_message>
<xml_diff>
--- a/rnaSample/rnaSample_Brown_11.25.19.xlsx
+++ b/rnaSample/rnaSample_Brown_11.25.19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/rnaSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3814ADF-82A4-1148-AA5C-9D9FEC2815A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFFC4D4-D3E0-AC41-966C-A0FADDD616ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19700" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="13">
   <si>
     <t>harvestDate</t>
   </si>
@@ -67,15 +67,15 @@
   </si>
   <si>
     <t>TRIzol</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -123,7 +123,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:L1048576"/>
+      <selection activeCell="H3" sqref="H3:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,8 +515,8 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="b">
-        <v>0</v>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -558,8 +558,8 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4" t="b">
-        <v>0</v>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -584,8 +584,8 @@
       <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4" t="b">
-        <v>0</v>
+      <c r="H4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -610,8 +610,8 @@
       <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4" t="b">
-        <v>0</v>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -636,8 +636,8 @@
       <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="4" t="b">
-        <v>0</v>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -662,8 +662,8 @@
       <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4" t="b">
-        <v>0</v>
+      <c r="H7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -688,8 +688,8 @@
       <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="4" t="b">
-        <v>0</v>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -714,8 +714,8 @@
       <c r="G9" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="4" t="b">
-        <v>0</v>
+      <c r="H9" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -740,8 +740,8 @@
       <c r="G10" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="4" t="b">
-        <v>0</v>
+      <c r="H10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -766,8 +766,8 @@
       <c r="G11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="4" t="b">
-        <v>0</v>
+      <c r="H11" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -792,8 +792,8 @@
       <c r="G12" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="4" t="b">
-        <v>0</v>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
@@ -818,8 +818,8 @@
       <c r="G13" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="4" t="b">
-        <v>0</v>
+      <c r="H13" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -844,8 +844,8 @@
       <c r="G14" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="4" t="b">
-        <v>0</v>
+      <c r="H14" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
@@ -870,8 +870,8 @@
       <c r="G15" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="4" t="b">
-        <v>0</v>
+      <c r="H15" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -896,8 +896,8 @@
       <c r="G16" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="4" t="b">
-        <v>0</v>
+      <c r="H16" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -922,8 +922,8 @@
       <c r="G17" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="4" t="b">
-        <v>0</v>
+      <c r="H17" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -948,8 +948,8 @@
       <c r="G18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="4" t="b">
-        <v>0</v>
+      <c r="H18" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -974,8 +974,8 @@
       <c r="G19" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="4" t="b">
-        <v>0</v>
+      <c r="H19" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1000,8 +1000,8 @@
       <c r="G20" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="4" t="b">
-        <v>0</v>
+      <c r="H20" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1026,8 +1026,8 @@
       <c r="G21" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="4" t="b">
-        <v>0</v>
+      <c r="H21" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1052,8 +1052,8 @@
       <c r="G22" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="4" t="b">
-        <v>0</v>
+      <c r="H22" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1078,8 +1078,8 @@
       <c r="G23" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="4" t="b">
-        <v>0</v>
+      <c r="H23" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1104,8 +1104,8 @@
       <c r="G24" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="4" t="b">
-        <v>0</v>
+      <c r="H24" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1130,8 +1130,8 @@
       <c r="G25" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="4" t="b">
-        <v>0</v>
+      <c r="H25" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1156,8 +1156,8 @@
       <c r="G26" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="4" t="b">
-        <v>0</v>
+      <c r="H26" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1182,8 +1182,8 @@
       <c r="G27" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="4" t="b">
-        <v>0</v>
+      <c r="H27" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>